<commit_message>
Added Molten Salt Storage.  Also fixed bug in battery calc
</commit_message>
<xml_diff>
--- a/Macro/Reference.xlsx
+++ b/Macro/Reference.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7cd0e7a053322a97/Documents/GenAtomic/Optimize/Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{19D1B901-19A4-4F5C-BD17-7EB35D9B857C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{322C973F-A448-4861-91F6-67C7CE8EFBA3}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{19D1B901-19A4-4F5C-BD17-7EB35D9B857C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BD6F1C8-F9B9-482B-A016-A18E21802BD9}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="9437" xr2:uid="{C81145A1-E574-4696-BBD3-79E862FF097E}"/>
   </bookViews>
@@ -680,7 +680,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
@@ -760,14 +760,14 @@
         <v>11</v>
       </c>
       <c r="I2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
         <v>39</v>
       </c>
       <c r="K2">
         <f>_1st_ref</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -802,7 +802,7 @@
       </c>
       <c r="K3">
         <f>K2+Param_Count</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -837,7 +837,7 @@
       </c>
       <c r="K4">
         <f>K3+Param_Count</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L4">
         <v>3</v>
@@ -872,7 +872,7 @@
       </c>
       <c r="K5">
         <f>K4+Param_Count</f>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -907,7 +907,7 @@
       </c>
       <c r="K6">
         <f>K5+Param_Count</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L6">
         <v>5</v>
@@ -941,7 +941,7 @@
       </c>
       <c r="K7">
         <f>K6+Param_Count</f>
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L7">
         <v>6</v>

</xml_diff>

<commit_message>
Fixed bug in multiplier algorithm.  Not sure why Cheap_Nuclear worked right?
</commit_message>
<xml_diff>
--- a/Macro/Reference.xlsx
+++ b/Macro/Reference.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7cd0e7a053322a97/Documents/GenAtomic/Optimize/Macro/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cliff\OneDrive\Documents\GenAtomic\Optimize\Macro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{19D1B901-19A4-4F5C-BD17-7EB35D9B857C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BD6F1C8-F9B9-482B-A016-A18E21802BD9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5513D7A9-1C9D-462E-AC7D-391C43331B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="9437" xr2:uid="{C81145A1-E574-4696-BBD3-79E862FF097E}"/>
   </bookViews>
@@ -17,6 +17,14 @@
   </sheets>
   <definedNames>
     <definedName name="_1st_ref">Reference!$I$2</definedName>
+    <definedName name="Analysis_Case2Filename">Reference!$S$2:$T$5</definedName>
+    <definedName name="Analysis2Long">Reference!$M$2:$N$4</definedName>
+    <definedName name="Analysis2Short">Reference!$N$2:$O$4</definedName>
+    <definedName name="Case2Long">Reference!$P$2:$Q$5</definedName>
+    <definedName name="Case2Short">Reference!$Q$2:$R$5</definedName>
+    <definedName name="CO2_Constant">Reference!$U$2:$U$7</definedName>
+    <definedName name="CO2_Per_Year">Reference!$V$2:$V$7</definedName>
+    <definedName name="Dir2Long">Reference!$M$2:$N$5</definedName>
     <definedName name="NRG_Selections">Reference!$J$2:$J$8</definedName>
     <definedName name="NRG_Table">Reference!$J$2:$L$8</definedName>
     <definedName name="Param_Count">Reference!$H$2</definedName>
@@ -25,6 +33,7 @@
     <definedName name="Region_abbr">Reference!$D$10</definedName>
     <definedName name="Region_lookup">Reference!$A$2:$B$15</definedName>
     <definedName name="Regions">Reference!$A$2:$A$15</definedName>
+    <definedName name="Sub2Long">Reference!$P$2:$Q$6</definedName>
     <definedName name="To_Long">Reference!$B$2:$C$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -106,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
   <si>
     <t>Texas</t>
   </si>
@@ -237,18 +246,9 @@
     <t>Entire US</t>
   </si>
   <si>
-    <t>Be Sure To Match Compare_Template.xlsx</t>
-  </si>
-  <si>
-    <t>NRG_Table</t>
-  </si>
-  <si>
     <t>1st ref</t>
   </si>
   <si>
-    <t>Parm_Count</t>
-  </si>
-  <si>
     <t>Mults</t>
   </si>
   <si>
@@ -258,9 +258,6 @@
     <t>Params</t>
   </si>
   <si>
-    <t>Regions_abbrs</t>
-  </si>
-  <si>
     <t>Regions</t>
   </si>
   <si>
@@ -274,6 +271,96 @@
   </si>
   <si>
     <t>Offset</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Nominal</t>
+  </si>
+  <si>
+    <t>Cheap_Nuclear</t>
+  </si>
+  <si>
+    <t>Reduced Nuclear Capital Cost</t>
+  </si>
+  <si>
+    <t>3_Qtr_Cap</t>
+  </si>
+  <si>
+    <t>By 25%</t>
+  </si>
+  <si>
+    <t>Half_Cap</t>
+  </si>
+  <si>
+    <t>In Half</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Fast_Build</t>
+  </si>
+  <si>
+    <t>Increase Max Build Rate All NRGs</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Double_All</t>
+  </si>
+  <si>
+    <t>By 2x</t>
+  </si>
+  <si>
+    <t>Nuke_Cap$_0.5_1</t>
+  </si>
+  <si>
+    <t>Nuke_Cap$_0.75_1</t>
+  </si>
+  <si>
+    <t>Regions abbrs</t>
+  </si>
+  <si>
+    <t>Parm Count</t>
+  </si>
+  <si>
+    <t>NRG Table</t>
+  </si>
+  <si>
+    <t>Analysis Long</t>
+  </si>
+  <si>
+    <t>Analysis Short</t>
+  </si>
+  <si>
+    <t>Case Long</t>
+  </si>
+  <si>
+    <t>Case Short</t>
+  </si>
+  <si>
+    <t>Analysis Case</t>
+  </si>
+  <si>
+    <t>FileName Extension</t>
+  </si>
+  <si>
+    <t>CO2 Constant</t>
+  </si>
+  <si>
+    <t>CO2 Per Year</t>
+  </si>
+  <si>
+    <t>-&lt;0&gt;-</t>
+  </si>
+  <si>
+    <t>Coal_Grow_2_1-Gas_Grow_2_1-Nuke_Grow_2_1-Solar_Grow_2_1-Batt_Grow_2_1-Wind_Grow_2_1</t>
   </si>
 </sst>
 </file>
@@ -330,14 +417,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,10 +443,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -677,70 +763,107 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200BB87E-1EE1-4FF4-A940-43E30C2581DF}">
   <sheetPr codeName="Sheet16"/>
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
   <cols>
-    <col min="1" max="3" width="12.07421875" customWidth="1"/>
-    <col min="4" max="4" width="14.69140625" customWidth="1"/>
-    <col min="5" max="5" width="1.65234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.265625" customWidth="1"/>
-    <col min="7" max="7" width="9.15234375" customWidth="1"/>
-    <col min="8" max="8" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="12.07421875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.69140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="1.65234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.265625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.15234375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="8.921875" style="2"/>
+    <col min="13" max="13" width="9.73046875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="15.73046875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.8828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.11328125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.9609375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="11.34375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="10.11328125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="19.8828125" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="8.921875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.85">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="str">
         <f>A1</f>
         <v>Regions</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -759,28 +882,58 @@
       <c r="H2" s="2">
         <v>11</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="2">
         <f>_1st_ref</f>
         <v>16</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A3" t="s">
+      <c r="M2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" s="2" t="str">
+        <f>M2</f>
+        <v>-&lt;0&gt;-</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="R2" s="2" t="str">
+        <f t="shared" ref="R2:R3" si="0">P2</f>
+        <v>-&lt;0&gt;-</v>
+      </c>
+      <c r="S2" s="2" t="str">
+        <f>M2 &amp; "_" &amp; P2</f>
+        <v>-&lt;0&gt;-_-&lt;0&gt;-</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="29.15" x14ac:dyDescent="0.85">
+      <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -796,26 +949,55 @@
         <f>1/1000000</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="2">
         <f>K2+Param_Count</f>
         <v>27</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A4" t="s">
+      <c r="M3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="2" t="str">
+        <f>M3</f>
+        <v>Default</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Default</v>
+      </c>
+      <c r="S3" s="2" t="str">
+        <f>M3 &amp; "_" &amp; P3</f>
+        <v>Default_Default</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0</v>
+      </c>
+      <c r="V3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="43.9" x14ac:dyDescent="0.85">
+      <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -831,26 +1013,58 @@
         <f>1/1000000</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="J4" t="s">
+      <c r="J4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="2">
         <f>K3+Param_Count</f>
         <v>38</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A5" t="s">
+      <c r="M4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" s="2" t="str">
+        <f t="shared" ref="O4:O5" si="1">M4</f>
+        <v>Cheap_Nuclear</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R4" s="2" t="str">
+        <f>P4</f>
+        <v>3_Qtr_Cap</v>
+      </c>
+      <c r="S4" s="2" t="str">
+        <f>M4 &amp; "_" &amp; P4</f>
+        <v>Cheap_Nuclear_3_Qtr_Cap</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="U4" s="2">
+        <v>100</v>
+      </c>
+      <c r="V4" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="43.9" x14ac:dyDescent="0.85">
+      <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -866,26 +1080,58 @@
         <f>1/1000</f>
         <v>1E-3</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="J5" t="s">
+      <c r="J5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="2">
         <f>K4+Param_Count</f>
         <v>49</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A6" t="s">
+      <c r="M5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Fast_Build</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R5" s="2" t="str">
+        <f>P5</f>
+        <v>Half_Cap</v>
+      </c>
+      <c r="S5" s="2" t="str">
+        <f>M4 &amp; "_" &amp; P5</f>
+        <v>Cheap_Nuclear_Half_Cap</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U5" s="2">
+        <v>200</v>
+      </c>
+      <c r="V5" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="87.45" x14ac:dyDescent="0.85">
+      <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -901,26 +1147,51 @@
         <f>1/1000</f>
         <v>1E-3</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="J6" t="s">
+      <c r="J6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="2">
         <f>K5+Param_Count</f>
         <v>60</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A7" t="s">
+      <c r="N6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R6" s="2" t="str">
+        <f>P6</f>
+        <v>Double_All</v>
+      </c>
+      <c r="S6" s="2" t="str">
+        <f>M5 &amp; "_" &amp; P6</f>
+        <v>Fast_Build_Double_All</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="U6" s="2">
+        <v>350</v>
+      </c>
+      <c r="V6" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -935,122 +1206,123 @@
       <c r="G7" s="2">
         <v>1</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="J7" t="s">
+      <c r="J7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="2">
         <f>K6+Param_Count</f>
         <v>71</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A8" t="s">
+      <c r="U7" s="2">
+        <v>500</v>
+      </c>
+      <c r="V7" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="J8" t="s">
-        <v>52</v>
-      </c>
-      <c r="L8">
+      <c r="J8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A9" t="s">
+    <row r="9" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A10" t="s">
+    <row r="10" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A11" t="s">
+    <row r="11" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A12" t="s">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.85">
+      <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A13" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.85">
+      <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A14" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.85">
+      <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.85">
-      <c r="A15" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.85">
+      <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.85"/>
+      <c r="O15" s="2">
+        <f t="shared" ref="O15" si="2">M15</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
More cleanup of initial state of graphs
</commit_message>
<xml_diff>
--- a/Macro/Reference.xlsx
+++ b/Macro/Reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cliff\OneDrive\Documents\GenAtomic\Optimize\Macro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5513D7A9-1C9D-462E-AC7D-391C43331B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5AB2A5-9B72-4287-8C51-580615A3FE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="9437" xr2:uid="{C81145A1-E574-4696-BBD3-79E862FF097E}"/>
   </bookViews>
@@ -17,14 +17,14 @@
   </sheets>
   <definedNames>
     <definedName name="_1st_ref">Reference!$I$2</definedName>
-    <definedName name="Analysis_Case2Filename">Reference!$S$2:$T$5</definedName>
-    <definedName name="Analysis2Long">Reference!$M$2:$N$4</definedName>
-    <definedName name="Analysis2Short">Reference!$N$2:$O$4</definedName>
-    <definedName name="Case2Long">Reference!$P$2:$Q$5</definedName>
-    <definedName name="Case2Short">Reference!$Q$2:$R$5</definedName>
+    <definedName name="Analysis_Case2Filename">Reference!$S$2:$T$99</definedName>
+    <definedName name="Analysis2Long">Reference!$M$2:$N$99</definedName>
+    <definedName name="Analysis2Short">Reference!$N$2:$O$99</definedName>
+    <definedName name="Case2Long">Reference!$P$2:$Q$99</definedName>
+    <definedName name="Case2Short">Reference!$Q$2:$R$99</definedName>
     <definedName name="CO2_Constant">Reference!$U$2:$U$7</definedName>
     <definedName name="CO2_Per_Year">Reference!$V$2:$V$7</definedName>
-    <definedName name="Dir2Long">Reference!$M$2:$N$5</definedName>
+    <definedName name="Dir2Long">Reference!$M$2:$N$99</definedName>
     <definedName name="NRG_Selections">Reference!$J$2:$J$8</definedName>
     <definedName name="NRG_Table">Reference!$J$2:$L$8</definedName>
     <definedName name="Param_Count">Reference!$H$2</definedName>
@@ -33,7 +33,7 @@
     <definedName name="Region_abbr">Reference!$D$10</definedName>
     <definedName name="Region_lookup">Reference!$A$2:$B$15</definedName>
     <definedName name="Regions">Reference!$A$2:$A$15</definedName>
-    <definedName name="Sub2Long">Reference!$P$2:$Q$6</definedName>
+    <definedName name="Sub2Long">Reference!$P$2:$Q$99</definedName>
     <definedName name="To_Long">Reference!$B$2:$C$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -765,7 +765,7 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K2" workbookViewId="0">
       <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
@@ -1240,7 +1240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.85">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.85">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.85">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Shortened paths. Optimize/Macro/../Library -> Optimize/Library.  Cases where we have one dexcriptor for each NRG, went to 1 descriptor for All_NRG
</commit_message>
<xml_diff>
--- a/Macro/Reference.xlsx
+++ b/Macro/Reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cliff\OneDrive\Documents\GenAtomic\Optimize\Macro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5AB2A5-9B72-4287-8C51-580615A3FE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DF56C3-7C3C-489A-9BD7-192C5582A633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="9437" xr2:uid="{C81145A1-E574-4696-BBD3-79E862FF097E}"/>
   </bookViews>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="85">
   <si>
     <t>Texas</t>
   </si>
@@ -309,9 +309,6 @@
     <t>Increase Max Build Rate All NRGs</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>Double_All</t>
   </si>
   <si>
@@ -360,7 +357,19 @@
     <t>-&lt;0&gt;-</t>
   </si>
   <si>
-    <t>Coal_Grow_2_1-Gas_Grow_2_1-Nuke_Grow_2_1-Solar_Grow_2_1-Batt_Grow_2_1-Wind_Grow_2_1</t>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>5%_Per_Year</t>
+  </si>
+  <si>
+    <t>5% Cheaper Per Year</t>
+  </si>
+  <si>
+    <t>Nuke_Cap$_1_0.95</t>
+  </si>
+  <si>
+    <t>All_NRG_Grow_2_1</t>
   </si>
 </sst>
 </file>
@@ -766,7 +775,7 @@
   <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K2" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
@@ -794,7 +803,7 @@
         <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="str">
         <f>A1</f>
@@ -811,13 +820,13 @@
         <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>50</v>
@@ -829,31 +838,31 @@
         <v>52</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>61</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
@@ -896,20 +905,20 @@
         <v>1</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O2" s="2" t="str">
         <f>M2</f>
         <v>-&lt;0&gt;-</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R2" s="2" t="str">
         <f t="shared" ref="R2:R3" si="0">P2</f>
@@ -920,10 +929,10 @@
         <v>-&lt;0&gt;-_-&lt;0&gt;-</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="29.15" x14ac:dyDescent="0.85">
@@ -1030,7 +1039,7 @@
         <v>56</v>
       </c>
       <c r="O4" s="2" t="str">
-        <f t="shared" ref="O4:O5" si="1">M4</f>
+        <f t="shared" ref="O4:O6" si="1">M4</f>
         <v>Cheap_Nuclear</v>
       </c>
       <c r="P4" s="2" t="s">
@@ -1048,7 +1057,7 @@
         <v>Cheap_Nuclear_3_Qtr_Cap</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U4" s="2">
         <v>100</v>
@@ -1115,7 +1124,7 @@
         <v>Cheap_Nuclear_Half_Cap</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U5" s="2">
         <v>200</v>
@@ -1124,7 +1133,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="87.45" x14ac:dyDescent="0.85">
+    <row r="6" spans="1:22" ht="29.15" x14ac:dyDescent="0.85">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1157,14 +1166,21 @@
       <c r="L6" s="2">
         <v>5</v>
       </c>
+      <c r="M6" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="N6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Debug</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="R6" s="2" t="str">
         <f>P6</f>
@@ -1175,7 +1191,7 @@
         <v>Fast_Build_Double_All</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="U6" s="2">
         <v>350</v>
@@ -1184,7 +1200,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
+    <row r="7" spans="1:22" ht="43.9" x14ac:dyDescent="0.85">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -1216,6 +1232,23 @@
       <c r="L7" s="2">
         <v>6</v>
       </c>
+      <c r="P7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="R7" s="2" t="str">
+        <f>P7</f>
+        <v>5%_Per_Year</v>
+      </c>
+      <c r="S7" s="2" t="str">
+        <f>M4 &amp; "_" &amp;P7</f>
+        <v>Cheap_Nuclear_5%_Per_Year</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="U7" s="2">
         <v>500</v>
       </c>
@@ -1223,7 +1256,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
+    <row r="8" spans="1:22" ht="29.15" x14ac:dyDescent="0.85">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1239,8 +1272,15 @@
       <c r="L8" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.85">
+      <c r="S8" s="2" t="str">
+        <f>M6 &amp; "_" &amp; P5</f>
+        <v>Debug_Half_Cap</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Got rid of Alias stuff
</commit_message>
<xml_diff>
--- a/Macro/Reference.xlsx
+++ b/Macro/Reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cliff\OneDrive\Documents\GenAtomic\Optimize\Macro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DF56C3-7C3C-489A-9BD7-192C5582A633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A13CEED-ED1C-4E66-9F24-974E759A6993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="9437" xr2:uid="{C81145A1-E574-4696-BBD3-79E862FF097E}"/>
   </bookViews>
@@ -17,14 +17,14 @@
   </sheets>
   <definedNames>
     <definedName name="_1st_ref">Reference!$I$2</definedName>
-    <definedName name="Analysis_Case2Filename">Reference!$S$2:$T$99</definedName>
-    <definedName name="Analysis2Long">Reference!$M$2:$N$99</definedName>
-    <definedName name="Analysis2Short">Reference!$N$2:$O$99</definedName>
-    <definedName name="Case2Long">Reference!$P$2:$Q$99</definedName>
-    <definedName name="Case2Short">Reference!$Q$2:$R$99</definedName>
-    <definedName name="CO2_Constant">Reference!$U$2:$U$7</definedName>
-    <definedName name="CO2_Per_Year">Reference!$V$2:$V$7</definedName>
-    <definedName name="Dir2Long">Reference!$M$2:$N$99</definedName>
+    <definedName name="Analysis_Case2Filename">Reference!#REF!</definedName>
+    <definedName name="Analysis2Long">Reference!#REF!</definedName>
+    <definedName name="Analysis2Short">Reference!#REF!</definedName>
+    <definedName name="Case2Long">Reference!#REF!</definedName>
+    <definedName name="Case2Short">Reference!#REF!</definedName>
+    <definedName name="CO2_Constant">Reference!#REF!</definedName>
+    <definedName name="CO2_Per_Year">Reference!#REF!</definedName>
+    <definedName name="Dir2Long">Reference!#REF!</definedName>
     <definedName name="NRG_Selections">Reference!$J$2:$J$8</definedName>
     <definedName name="NRG_Table">Reference!$J$2:$L$8</definedName>
     <definedName name="Param_Count">Reference!$H$2</definedName>
@@ -33,7 +33,7 @@
     <definedName name="Region_abbr">Reference!$D$10</definedName>
     <definedName name="Region_lookup">Reference!$A$2:$B$15</definedName>
     <definedName name="Regions">Reference!$A$2:$A$15</definedName>
-    <definedName name="Sub2Long">Reference!$P$2:$Q$99</definedName>
+    <definedName name="Sub2Long">Reference!#REF!</definedName>
     <definedName name="To_Long">Reference!$B$2:$C$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>Texas</t>
   </si>
@@ -273,54 +273,6 @@
     <t>Offset</t>
   </si>
   <si>
-    <t>Analysis</t>
-  </si>
-  <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>Nominal</t>
-  </si>
-  <si>
-    <t>Cheap_Nuclear</t>
-  </si>
-  <si>
-    <t>Reduced Nuclear Capital Cost</t>
-  </si>
-  <si>
-    <t>3_Qtr_Cap</t>
-  </si>
-  <si>
-    <t>By 25%</t>
-  </si>
-  <si>
-    <t>Half_Cap</t>
-  </si>
-  <si>
-    <t>In Half</t>
-  </si>
-  <si>
-    <t>Case</t>
-  </si>
-  <si>
-    <t>Fast_Build</t>
-  </si>
-  <si>
-    <t>Increase Max Build Rate All NRGs</t>
-  </si>
-  <si>
-    <t>Double_All</t>
-  </si>
-  <si>
-    <t>By 2x</t>
-  </si>
-  <si>
-    <t>Nuke_Cap$_0.5_1</t>
-  </si>
-  <si>
-    <t>Nuke_Cap$_0.75_1</t>
-  </si>
-  <si>
     <t>Regions abbrs</t>
   </si>
   <si>
@@ -328,48 +280,6 @@
   </si>
   <si>
     <t>NRG Table</t>
-  </si>
-  <si>
-    <t>Analysis Long</t>
-  </si>
-  <si>
-    <t>Analysis Short</t>
-  </si>
-  <si>
-    <t>Case Long</t>
-  </si>
-  <si>
-    <t>Case Short</t>
-  </si>
-  <si>
-    <t>Analysis Case</t>
-  </si>
-  <si>
-    <t>FileName Extension</t>
-  </si>
-  <si>
-    <t>CO2 Constant</t>
-  </si>
-  <si>
-    <t>CO2 Per Year</t>
-  </si>
-  <si>
-    <t>-&lt;0&gt;-</t>
-  </si>
-  <si>
-    <t>Debug</t>
-  </si>
-  <si>
-    <t>5%_Per_Year</t>
-  </si>
-  <si>
-    <t>5% Cheaper Per Year</t>
-  </si>
-  <si>
-    <t>Nuke_Cap$_1_0.95</t>
-  </si>
-  <si>
-    <t>All_NRG_Grow_2_1</t>
   </si>
 </sst>
 </file>
@@ -426,15 +336,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -772,10 +679,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200BB87E-1EE1-4FF4-A940-43E30C2581DF}">
   <sheetPr codeName="Sheet16"/>
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
@@ -786,24 +693,15 @@
     <col min="6" max="6" width="8.265625" style="2" customWidth="1"/>
     <col min="7" max="7" width="9.15234375" style="2" customWidth="1"/>
     <col min="8" max="8" width="10.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="8.921875" style="2"/>
-    <col min="13" max="13" width="9.73046875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="15.73046875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.8828125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.11328125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="9.9609375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="11.34375" style="2" customWidth="1"/>
-    <col min="19" max="19" width="10.11328125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="19.8828125" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="8.921875" style="2"/>
+    <col min="9" max="16384" width="8.921875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.85">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="str">
         <f>A1</f>
@@ -820,13 +718,13 @@
         <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>50</v>
@@ -834,38 +732,8 @@
       <c r="L1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.85">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -904,38 +772,8 @@
       <c r="L2" s="2">
         <v>1</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="O2" s="2" t="str">
-        <f>M2</f>
-        <v>-&lt;0&gt;-</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="R2" s="2" t="str">
-        <f t="shared" ref="R2:R3" si="0">P2</f>
-        <v>-&lt;0&gt;-</v>
-      </c>
-      <c r="S2" s="2" t="str">
-        <f>M2 &amp; "_" &amp; P2</f>
-        <v>-&lt;0&gt;-_-&lt;0&gt;-</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="29.15" x14ac:dyDescent="0.85">
+    </row>
+    <row r="3" spans="1:12" ht="29.15" x14ac:dyDescent="0.85">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -968,38 +806,8 @@
       <c r="L3" s="2">
         <v>2</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="2" t="str">
-        <f>M3</f>
-        <v>Default</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="R3" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>Default</v>
-      </c>
-      <c r="S3" s="2" t="str">
-        <f>M3 &amp; "_" &amp; P3</f>
-        <v>Default_Default</v>
-      </c>
-      <c r="U3" s="2">
-        <v>0</v>
-      </c>
-      <c r="V3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="43.9" x14ac:dyDescent="0.85">
+    </row>
+    <row r="4" spans="1:12" ht="43.9" x14ac:dyDescent="0.85">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -1032,41 +840,8 @@
       <c r="L4" s="2">
         <v>3</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="2" t="str">
-        <f t="shared" ref="O4:O6" si="1">M4</f>
-        <v>Cheap_Nuclear</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="R4" s="2" t="str">
-        <f>P4</f>
-        <v>3_Qtr_Cap</v>
-      </c>
-      <c r="S4" s="2" t="str">
-        <f>M4 &amp; "_" &amp; P4</f>
-        <v>Cheap_Nuclear_3_Qtr_Cap</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="U4" s="2">
-        <v>100</v>
-      </c>
-      <c r="V4" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="43.9" x14ac:dyDescent="0.85">
+    </row>
+    <row r="5" spans="1:12" ht="43.9" x14ac:dyDescent="0.85">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1099,41 +874,8 @@
       <c r="L5" s="2">
         <v>4</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="O5" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Fast_Build</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="R5" s="2" t="str">
-        <f>P5</f>
-        <v>Half_Cap</v>
-      </c>
-      <c r="S5" s="2" t="str">
-        <f>M4 &amp; "_" &amp; P5</f>
-        <v>Cheap_Nuclear_Half_Cap</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U5" s="2">
-        <v>200</v>
-      </c>
-      <c r="V5" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="29.15" x14ac:dyDescent="0.85">
+    </row>
+    <row r="6" spans="1:12" ht="29.15" x14ac:dyDescent="0.85">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1166,41 +908,8 @@
       <c r="L6" s="2">
         <v>5</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="O6" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Debug</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="R6" s="2" t="str">
-        <f>P6</f>
-        <v>Double_All</v>
-      </c>
-      <c r="S6" s="2" t="str">
-        <f>M5 &amp; "_" &amp; P6</f>
-        <v>Fast_Build_Double_All</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="U6" s="2">
-        <v>350</v>
-      </c>
-      <c r="V6" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="43.9" x14ac:dyDescent="0.85">
+    </row>
+    <row r="7" spans="1:12" ht="43.9" x14ac:dyDescent="0.85">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -1232,31 +941,8 @@
       <c r="L7" s="2">
         <v>6</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="R7" s="2" t="str">
-        <f>P7</f>
-        <v>5%_Per_Year</v>
-      </c>
-      <c r="S7" s="2" t="str">
-        <f>M4 &amp; "_" &amp;P7</f>
-        <v>Cheap_Nuclear_5%_Per_Year</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="U7" s="2">
-        <v>500</v>
-      </c>
-      <c r="V7" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="29.15" x14ac:dyDescent="0.85">
+    </row>
+    <row r="8" spans="1:12" ht="29.15" x14ac:dyDescent="0.85">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1272,15 +958,8 @@
       <c r="L8" s="2">
         <v>7</v>
       </c>
-      <c r="S8" s="2" t="str">
-        <f>M6 &amp; "_" &amp; P5</f>
-        <v>Debug_Half_Cap</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="14.65" x14ac:dyDescent="0.85">
+    </row>
+    <row r="9" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1292,7 +971,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.85">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.85">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1303,7 +982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.85">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.85">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1314,7 +993,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.85">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.85">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1325,7 +1004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.85">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.85">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -1336,7 +1015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.85">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.85">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1347,7 +1026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.85">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.85">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1355,10 +1034,6 @@
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O15" s="2">
-        <f t="shared" ref="O15" si="2">M15</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Got rid of #Refs left over from when I got rid of the Alias stuff
</commit_message>
<xml_diff>
--- a/Macro/Reference.xlsx
+++ b/Macro/Reference.xlsx
@@ -1,30 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cliff\OneDrive\Documents\GenAtomic\Optimize\Macro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A13CEED-ED1C-4E66-9F24-974E759A6993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AECB17-B799-44EB-B6FF-C266041B7D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="9437" xr2:uid="{C81145A1-E574-4696-BBD3-79E862FF097E}"/>
+    <workbookView xWindow="2644" yWindow="600" windowWidth="12343" windowHeight="6677" xr2:uid="{C81145A1-E574-4696-BBD3-79E862FF097E}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_1st_ref">Reference!$I$2</definedName>
-    <definedName name="Analysis_Case2Filename">Reference!#REF!</definedName>
-    <definedName name="Analysis2Long">Reference!#REF!</definedName>
-    <definedName name="Analysis2Short">Reference!#REF!</definedName>
-    <definedName name="Case2Long">Reference!#REF!</definedName>
-    <definedName name="Case2Short">Reference!#REF!</definedName>
-    <definedName name="CO2_Constant">Reference!#REF!</definedName>
-    <definedName name="CO2_Per_Year">Reference!#REF!</definedName>
-    <definedName name="Dir2Long">Reference!#REF!</definedName>
     <definedName name="NRG_Selections">Reference!$J$2:$J$8</definedName>
     <definedName name="NRG_Table">Reference!$J$2:$L$8</definedName>
     <definedName name="Param_Count">Reference!$H$2</definedName>
@@ -33,7 +25,6 @@
     <definedName name="Region_abbr">Reference!$D$10</definedName>
     <definedName name="Region_lookup">Reference!$A$2:$B$15</definedName>
     <definedName name="Regions">Reference!$A$2:$A$15</definedName>
-    <definedName name="Sub2Long">Reference!#REF!</definedName>
     <definedName name="To_Long">Reference!$B$2:$C$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -681,7 +672,7 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
@@ -733,7 +724,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.85">
+    <row r="2" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -841,7 +832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="43.9" x14ac:dyDescent="0.85">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.85">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -875,7 +866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="29.15" x14ac:dyDescent="0.85">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.85">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -909,7 +900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="43.9" x14ac:dyDescent="0.85">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.85">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -942,7 +933,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="29.15" x14ac:dyDescent="0.85">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.85">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -959,7 +950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.85">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>